<commit_message>
agrego json de categoria issue 8
</commit_message>
<xml_diff>
--- a/Testing/Tests - Casos de Prueba - Spring 1.xlsx
+++ b/Testing/Tests - Casos de Prueba - Spring 1.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="60">
   <si>
     <t>ID</t>
   </si>
@@ -204,7 +204,7 @@
     <t>Ser redirigido al home de la app con mi usuario</t>
   </si>
   <si>
-    <t>Grupo 2</t>
+    <t>Pato Alloco</t>
   </si>
 </sst>
 </file>
@@ -422,102 +422,102 @@
   </cellStyleXfs>
   <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -800,8 +800,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I31" sqref="I31"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -819,639 +819,567 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="2" t="s">
+      <c r="F1" s="35"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="J1" s="30" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="7"/>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="9" t="s">
+      <c r="A2" s="31"/>
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="24" t="s">
+      <c r="F2" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="G2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="7"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="31"/>
     </row>
     <row r="3" spans="1:10" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="11">
+      <c r="A3" s="23">
         <v>1</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="17" t="s">
+      <c r="C3" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="19" t="s">
+      <c r="D3" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="23">
+      <c r="E3" s="7">
         <v>1</v>
       </c>
-      <c r="F3" s="25" t="s">
+      <c r="F3" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="13" t="s">
+      <c r="G3" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="H3" s="21"/>
-      <c r="I3" s="22" t="s">
+      <c r="H3" s="32"/>
+      <c r="I3" s="27" t="s">
         <v>59</v>
       </c>
-      <c r="J3" s="17"/>
+      <c r="J3" s="16"/>
     </row>
     <row r="4" spans="1:10" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="14"/>
-      <c r="B4" s="18"/>
-      <c r="C4" s="18"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="12">
+      <c r="A4" s="24"/>
+      <c r="B4" s="17"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="3">
         <v>2</v>
       </c>
-      <c r="F4" s="15" t="s">
+      <c r="F4" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="G4" s="15" t="s">
+      <c r="G4" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="H4" s="18"/>
-      <c r="I4" s="20"/>
-      <c r="J4" s="18"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="26"/>
+      <c r="J4" s="17"/>
     </row>
     <row r="5" spans="1:10" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="14"/>
-      <c r="B5" s="18"/>
-      <c r="C5" s="18"/>
-      <c r="D5" s="20"/>
-      <c r="E5" s="12">
+      <c r="A5" s="24"/>
+      <c r="B5" s="17"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="26"/>
+      <c r="E5" s="3">
         <v>3</v>
       </c>
-      <c r="F5" s="16" t="s">
+      <c r="F5" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="G5" s="16"/>
-      <c r="H5" s="18"/>
-      <c r="I5" s="20"/>
-      <c r="J5" s="18"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="17"/>
+      <c r="I5" s="26"/>
+      <c r="J5" s="17"/>
     </row>
     <row r="6" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="14"/>
-      <c r="B6" s="18"/>
-      <c r="C6" s="18"/>
-      <c r="D6" s="20"/>
-      <c r="E6" s="12">
+      <c r="A6" s="24"/>
+      <c r="B6" s="17"/>
+      <c r="C6" s="17"/>
+      <c r="D6" s="26"/>
+      <c r="E6" s="3">
         <v>4</v>
       </c>
-      <c r="F6" s="26" t="s">
+      <c r="F6" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="G6" s="26" t="s">
+      <c r="G6" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="H6" s="18"/>
-      <c r="I6" s="20"/>
-      <c r="J6" s="18"/>
+      <c r="H6" s="17"/>
+      <c r="I6" s="26"/>
+      <c r="J6" s="17"/>
     </row>
     <row r="7" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="11">
+      <c r="A7" s="23">
         <v>2</v>
       </c>
-      <c r="B7" s="17" t="s">
+      <c r="B7" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="17" t="s">
+      <c r="C7" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="D7" s="19" t="s">
+      <c r="D7" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="E7" s="23">
+      <c r="E7" s="7">
         <v>1</v>
       </c>
-      <c r="F7" s="25" t="s">
+      <c r="F7" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="G7" s="27" t="s">
+      <c r="G7" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="H7" s="22"/>
-      <c r="I7" s="22" t="s">
+      <c r="H7" s="27"/>
+      <c r="I7" s="27" t="s">
         <v>59</v>
       </c>
-      <c r="J7" s="17"/>
+      <c r="J7" s="16"/>
     </row>
     <row r="8" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="14"/>
-      <c r="B8" s="18"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="20"/>
-      <c r="E8" s="23">
+      <c r="A8" s="24"/>
+      <c r="B8" s="17"/>
+      <c r="C8" s="17"/>
+      <c r="D8" s="26"/>
+      <c r="E8" s="7">
         <v>2</v>
       </c>
-      <c r="F8" s="27" t="s">
+      <c r="F8" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="G8" s="27" t="s">
+      <c r="G8" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="H8" s="20"/>
-      <c r="I8" s="20"/>
-      <c r="J8" s="18"/>
+      <c r="H8" s="26"/>
+      <c r="I8" s="26"/>
+      <c r="J8" s="17"/>
     </row>
     <row r="9" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A9" s="14"/>
-      <c r="B9" s="18"/>
-      <c r="C9" s="18"/>
-      <c r="D9" s="20"/>
-      <c r="E9" s="23">
+      <c r="A9" s="24"/>
+      <c r="B9" s="17"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="26"/>
+      <c r="E9" s="7">
         <v>3</v>
       </c>
-      <c r="F9" s="27" t="s">
+      <c r="F9" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="G9" s="27" t="s">
+      <c r="G9" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="H9" s="20"/>
-      <c r="I9" s="20"/>
-      <c r="J9" s="18"/>
+      <c r="H9" s="26"/>
+      <c r="I9" s="26"/>
+      <c r="J9" s="17"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="14"/>
-      <c r="B10" s="18"/>
-      <c r="C10" s="18"/>
-      <c r="D10" s="20"/>
-      <c r="E10" s="23">
+      <c r="A10" s="24"/>
+      <c r="B10" s="17"/>
+      <c r="C10" s="17"/>
+      <c r="D10" s="26"/>
+      <c r="E10" s="7">
         <v>4</v>
       </c>
-      <c r="F10" s="27" t="s">
+      <c r="F10" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="G10" s="27" t="s">
+      <c r="G10" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="H10" s="20"/>
-      <c r="I10" s="20"/>
-      <c r="J10" s="18"/>
+      <c r="H10" s="26"/>
+      <c r="I10" s="26"/>
+      <c r="J10" s="17"/>
     </row>
     <row r="11" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A11" s="11">
+      <c r="A11" s="23">
         <v>3</v>
       </c>
-      <c r="B11" s="17" t="s">
+      <c r="B11" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="C11" s="17" t="s">
+      <c r="C11" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="D11" s="19" t="s">
+      <c r="D11" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="E11" s="23">
+      <c r="E11" s="7">
         <v>1</v>
       </c>
-      <c r="F11" s="25" t="s">
+      <c r="F11" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="G11" s="27" t="s">
+      <c r="G11" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="H11" s="22"/>
-      <c r="I11" s="22" t="s">
+      <c r="H11" s="27"/>
+      <c r="I11" s="27" t="s">
         <v>59</v>
       </c>
-      <c r="J11" s="17"/>
+      <c r="J11" s="16"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="14"/>
-      <c r="B12" s="18"/>
-      <c r="C12" s="18"/>
-      <c r="D12" s="20"/>
-      <c r="E12" s="23">
+      <c r="A12" s="24"/>
+      <c r="B12" s="17"/>
+      <c r="C12" s="17"/>
+      <c r="D12" s="26"/>
+      <c r="E12" s="7">
         <v>2</v>
       </c>
-      <c r="F12" s="27" t="s">
+      <c r="F12" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="G12" s="27" t="s">
+      <c r="G12" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="H12" s="20"/>
-      <c r="I12" s="20"/>
-      <c r="J12" s="18"/>
+      <c r="H12" s="26"/>
+      <c r="I12" s="26"/>
+      <c r="J12" s="17"/>
     </row>
     <row r="13" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A13" s="14"/>
-      <c r="B13" s="18"/>
-      <c r="C13" s="18"/>
-      <c r="D13" s="20"/>
-      <c r="E13" s="23">
+      <c r="A13" s="24"/>
+      <c r="B13" s="17"/>
+      <c r="C13" s="17"/>
+      <c r="D13" s="26"/>
+      <c r="E13" s="7">
         <v>3</v>
       </c>
-      <c r="F13" s="27" t="s">
+      <c r="F13" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="G13" s="27" t="s">
+      <c r="G13" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="H13" s="20"/>
-      <c r="I13" s="20"/>
-      <c r="J13" s="18"/>
+      <c r="H13" s="26"/>
+      <c r="I13" s="26"/>
+      <c r="J13" s="17"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="14"/>
-      <c r="B14" s="18"/>
-      <c r="C14" s="18"/>
-      <c r="D14" s="20"/>
-      <c r="E14" s="23">
+      <c r="A14" s="24"/>
+      <c r="B14" s="17"/>
+      <c r="C14" s="17"/>
+      <c r="D14" s="26"/>
+      <c r="E14" s="7">
         <v>4</v>
       </c>
-      <c r="F14" s="27"/>
-      <c r="G14" s="27"/>
-      <c r="H14" s="20"/>
-      <c r="I14" s="20"/>
-      <c r="J14" s="18"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="26"/>
+      <c r="I14" s="26"/>
+      <c r="J14" s="17"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="11">
+      <c r="A15" s="23">
         <v>4</v>
       </c>
-      <c r="B15" s="17" t="s">
+      <c r="B15" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="C15" s="17" t="s">
+      <c r="C15" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="D15" s="19" t="s">
+      <c r="D15" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="E15" s="23">
+      <c r="E15" s="7">
         <v>1</v>
       </c>
-      <c r="F15" s="25" t="s">
+      <c r="F15" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="G15" s="27" t="s">
+      <c r="G15" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="H15" s="22"/>
-      <c r="I15" s="22" t="s">
+      <c r="H15" s="27"/>
+      <c r="I15" s="27" t="s">
         <v>59</v>
       </c>
-      <c r="J15" s="17"/>
+      <c r="J15" s="16"/>
     </row>
     <row r="16" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A16" s="14"/>
-      <c r="B16" s="18"/>
-      <c r="C16" s="18"/>
-      <c r="D16" s="20"/>
-      <c r="E16" s="23">
+      <c r="A16" s="24"/>
+      <c r="B16" s="17"/>
+      <c r="C16" s="17"/>
+      <c r="D16" s="26"/>
+      <c r="E16" s="7">
         <v>2</v>
       </c>
-      <c r="F16" s="27" t="s">
+      <c r="F16" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="G16" s="27" t="s">
+      <c r="G16" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="H16" s="20"/>
-      <c r="I16" s="20"/>
-      <c r="J16" s="18"/>
+      <c r="H16" s="26"/>
+      <c r="I16" s="26"/>
+      <c r="J16" s="17"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="14"/>
-      <c r="B17" s="18"/>
-      <c r="C17" s="18"/>
-      <c r="D17" s="20"/>
-      <c r="E17" s="23">
+      <c r="A17" s="24"/>
+      <c r="B17" s="17"/>
+      <c r="C17" s="17"/>
+      <c r="D17" s="26"/>
+      <c r="E17" s="7">
         <v>3</v>
       </c>
-      <c r="F17" s="27"/>
-      <c r="G17" s="27"/>
-      <c r="H17" s="20"/>
-      <c r="I17" s="20"/>
-      <c r="J17" s="18"/>
+      <c r="F17" s="11"/>
+      <c r="G17" s="11"/>
+      <c r="H17" s="26"/>
+      <c r="I17" s="26"/>
+      <c r="J17" s="17"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="14"/>
-      <c r="B18" s="18"/>
-      <c r="C18" s="18"/>
-      <c r="D18" s="20"/>
-      <c r="E18" s="23">
+      <c r="A18" s="24"/>
+      <c r="B18" s="17"/>
+      <c r="C18" s="17"/>
+      <c r="D18" s="26"/>
+      <c r="E18" s="7">
         <v>4</v>
       </c>
-      <c r="F18" s="27"/>
-      <c r="G18" s="27"/>
-      <c r="H18" s="20"/>
-      <c r="I18" s="20"/>
-      <c r="J18" s="18"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="11"/>
+      <c r="H18" s="26"/>
+      <c r="I18" s="26"/>
+      <c r="J18" s="17"/>
     </row>
     <row r="19" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="11">
+      <c r="A19" s="23">
         <v>5</v>
       </c>
-      <c r="B19" s="17" t="s">
+      <c r="B19" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="C19" s="17" t="s">
+      <c r="C19" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="D19" s="19" t="s">
+      <c r="D19" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="E19" s="23">
+      <c r="E19" s="7">
         <v>1</v>
       </c>
-      <c r="F19" s="28" t="s">
+      <c r="F19" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="G19" s="27" t="s">
+      <c r="G19" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="H19" s="22"/>
-      <c r="I19" s="22" t="s">
+      <c r="H19" s="27"/>
+      <c r="I19" s="27" t="s">
         <v>59</v>
       </c>
-      <c r="J19" s="17"/>
+      <c r="J19" s="16"/>
     </row>
     <row r="20" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A20" s="14"/>
-      <c r="B20" s="18"/>
-      <c r="C20" s="18"/>
-      <c r="D20" s="20"/>
-      <c r="E20" s="23">
+      <c r="A20" s="24"/>
+      <c r="B20" s="17"/>
+      <c r="C20" s="17"/>
+      <c r="D20" s="26"/>
+      <c r="E20" s="7">
         <v>2</v>
       </c>
-      <c r="F20" s="27" t="s">
+      <c r="F20" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="G20" s="27" t="s">
+      <c r="G20" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="H20" s="20"/>
-      <c r="I20" s="20"/>
-      <c r="J20" s="18"/>
+      <c r="H20" s="26"/>
+      <c r="I20" s="26"/>
+      <c r="J20" s="17"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="14"/>
-      <c r="B21" s="18"/>
-      <c r="C21" s="18"/>
-      <c r="D21" s="20"/>
-      <c r="E21" s="23">
+      <c r="A21" s="24"/>
+      <c r="B21" s="17"/>
+      <c r="C21" s="17"/>
+      <c r="D21" s="26"/>
+      <c r="E21" s="7">
         <v>3</v>
       </c>
-      <c r="F21" s="27"/>
-      <c r="G21" s="27"/>
-      <c r="H21" s="20"/>
-      <c r="I21" s="20"/>
-      <c r="J21" s="18"/>
+      <c r="F21" s="11"/>
+      <c r="G21" s="11"/>
+      <c r="H21" s="26"/>
+      <c r="I21" s="26"/>
+      <c r="J21" s="17"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="14"/>
-      <c r="B22" s="18"/>
-      <c r="C22" s="18"/>
-      <c r="D22" s="20"/>
-      <c r="E22" s="23">
+      <c r="A22" s="24"/>
+      <c r="B22" s="17"/>
+      <c r="C22" s="17"/>
+      <c r="D22" s="26"/>
+      <c r="E22" s="7">
         <v>4</v>
       </c>
-      <c r="F22" s="27"/>
-      <c r="G22" s="27"/>
-      <c r="H22" s="20"/>
-      <c r="I22" s="20"/>
-      <c r="J22" s="18"/>
+      <c r="F22" s="11"/>
+      <c r="G22" s="11"/>
+      <c r="H22" s="26"/>
+      <c r="I22" s="26"/>
+      <c r="J22" s="17"/>
     </row>
     <row r="23" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="11">
+      <c r="A23" s="23">
         <v>6</v>
       </c>
-      <c r="B23" s="17" t="s">
+      <c r="B23" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="C23" s="17" t="s">
+      <c r="C23" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="D23" s="19" t="s">
+      <c r="D23" s="25" t="s">
         <v>52</v>
       </c>
-      <c r="E23" s="23">
+      <c r="E23" s="7">
         <v>1</v>
       </c>
-      <c r="F23" s="28" t="s">
+      <c r="F23" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="G23" s="27" t="s">
+      <c r="G23" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="H23" s="22"/>
-      <c r="I23" s="22" t="s">
+      <c r="H23" s="27"/>
+      <c r="I23" s="27" t="s">
         <v>59</v>
       </c>
-      <c r="J23" s="17"/>
+      <c r="J23" s="16"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="14"/>
-      <c r="B24" s="18"/>
-      <c r="C24" s="18"/>
-      <c r="D24" s="20"/>
-      <c r="E24" s="23">
+      <c r="A24" s="24"/>
+      <c r="B24" s="17"/>
+      <c r="C24" s="17"/>
+      <c r="D24" s="26"/>
+      <c r="E24" s="7">
         <v>2</v>
       </c>
-      <c r="F24" s="27" t="s">
+      <c r="F24" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="G24" s="27" t="s">
+      <c r="G24" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="H24" s="20"/>
-      <c r="I24" s="20"/>
-      <c r="J24" s="18"/>
+      <c r="H24" s="26"/>
+      <c r="I24" s="26"/>
+      <c r="J24" s="17"/>
     </row>
     <row r="25" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A25" s="14"/>
-      <c r="B25" s="18"/>
-      <c r="C25" s="18"/>
-      <c r="D25" s="20"/>
-      <c r="E25" s="23">
+      <c r="A25" s="24"/>
+      <c r="B25" s="17"/>
+      <c r="C25" s="17"/>
+      <c r="D25" s="26"/>
+      <c r="E25" s="7">
         <v>3</v>
       </c>
-      <c r="F25" s="27" t="s">
+      <c r="F25" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="G25" s="27" t="s">
+      <c r="G25" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="H25" s="20"/>
-      <c r="I25" s="20"/>
-      <c r="J25" s="18"/>
+      <c r="H25" s="26"/>
+      <c r="I25" s="26"/>
+      <c r="J25" s="17"/>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="14"/>
-      <c r="B26" s="18"/>
-      <c r="C26" s="18"/>
-      <c r="D26" s="20"/>
-      <c r="E26" s="29">
+      <c r="A26" s="24"/>
+      <c r="B26" s="17"/>
+      <c r="C26" s="17"/>
+      <c r="D26" s="26"/>
+      <c r="E26" s="13">
         <v>4</v>
       </c>
-      <c r="F26" s="30"/>
-      <c r="G26" s="30"/>
-      <c r="H26" s="20"/>
-      <c r="I26" s="20"/>
-      <c r="J26" s="18"/>
-    </row>
-    <row r="27" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" s="31">
-        <v>7</v>
-      </c>
-      <c r="B27" s="32" t="s">
-        <v>50</v>
-      </c>
-      <c r="C27" s="32" t="s">
-        <v>51</v>
-      </c>
-      <c r="D27" s="32" t="s">
-        <v>52</v>
-      </c>
-      <c r="E27" s="33">
-        <v>1</v>
-      </c>
-      <c r="F27" s="28" t="s">
-        <v>53</v>
-      </c>
-      <c r="G27" s="27" t="s">
-        <v>54</v>
-      </c>
-      <c r="H27" s="34"/>
-      <c r="I27" s="34" t="s">
-        <v>59</v>
-      </c>
-      <c r="J27" s="32"/>
+      <c r="F26" s="14"/>
+      <c r="G26" s="14"/>
+      <c r="H26" s="26"/>
+      <c r="I26" s="26"/>
+      <c r="J26" s="17"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" s="18"/>
+      <c r="B27" s="20"/>
+      <c r="C27" s="20"/>
+      <c r="D27" s="20"/>
+      <c r="E27" s="15"/>
+      <c r="F27" s="12"/>
+      <c r="G27" s="11"/>
+      <c r="H27" s="22"/>
+      <c r="I27" s="22"/>
+      <c r="J27" s="20"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" s="35"/>
-      <c r="B28" s="36"/>
-      <c r="C28" s="36"/>
-      <c r="D28" s="36"/>
-      <c r="E28" s="33">
-        <v>2</v>
-      </c>
-      <c r="F28" s="27" t="s">
-        <v>55</v>
-      </c>
-      <c r="G28" s="27" t="s">
-        <v>56</v>
-      </c>
-      <c r="H28" s="36"/>
-      <c r="I28" s="36"/>
-      <c r="J28" s="36"/>
-    </row>
-    <row r="29" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A29" s="35"/>
-      <c r="B29" s="36"/>
-      <c r="C29" s="36"/>
-      <c r="D29" s="36"/>
-      <c r="E29" s="33">
-        <v>3</v>
-      </c>
-      <c r="F29" s="27" t="s">
-        <v>57</v>
-      </c>
-      <c r="G29" s="27" t="s">
-        <v>58</v>
-      </c>
-      <c r="H29" s="36"/>
-      <c r="I29" s="36"/>
-      <c r="J29" s="36"/>
+      <c r="A28" s="19"/>
+      <c r="B28" s="21"/>
+      <c r="C28" s="21"/>
+      <c r="D28" s="21"/>
+      <c r="E28" s="15"/>
+      <c r="F28" s="11"/>
+      <c r="G28" s="11"/>
+      <c r="H28" s="21"/>
+      <c r="I28" s="21"/>
+      <c r="J28" s="21"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" s="19"/>
+      <c r="B29" s="21"/>
+      <c r="C29" s="21"/>
+      <c r="D29" s="21"/>
+      <c r="E29" s="15"/>
+      <c r="F29" s="11"/>
+      <c r="G29" s="11"/>
+      <c r="H29" s="21"/>
+      <c r="I29" s="21"/>
+      <c r="J29" s="21"/>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" s="35"/>
-      <c r="B30" s="36"/>
-      <c r="C30" s="36"/>
-      <c r="D30" s="36"/>
-      <c r="E30" s="33">
-        <v>4</v>
-      </c>
-      <c r="F30" s="27"/>
-      <c r="G30" s="27"/>
-      <c r="H30" s="36"/>
-      <c r="I30" s="36"/>
-      <c r="J30" s="36"/>
+      <c r="A30" s="19"/>
+      <c r="B30" s="21"/>
+      <c r="C30" s="21"/>
+      <c r="D30" s="21"/>
+      <c r="E30" s="15"/>
+      <c r="F30" s="11"/>
+      <c r="G30" s="11"/>
+      <c r="H30" s="21"/>
+      <c r="I30" s="21"/>
+      <c r="J30" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="57">
-    <mergeCell ref="J23:J26"/>
-    <mergeCell ref="A27:A30"/>
-    <mergeCell ref="B27:B30"/>
-    <mergeCell ref="C27:C30"/>
-    <mergeCell ref="D27:D30"/>
-    <mergeCell ref="H27:H30"/>
-    <mergeCell ref="I27:I30"/>
-    <mergeCell ref="J27:J30"/>
-    <mergeCell ref="A23:A26"/>
-    <mergeCell ref="B23:B26"/>
-    <mergeCell ref="C23:C26"/>
-    <mergeCell ref="D23:D26"/>
-    <mergeCell ref="H23:H26"/>
-    <mergeCell ref="I23:I26"/>
-    <mergeCell ref="J15:J18"/>
-    <mergeCell ref="A19:A22"/>
-    <mergeCell ref="B19:B22"/>
-    <mergeCell ref="C19:C22"/>
-    <mergeCell ref="D19:D22"/>
-    <mergeCell ref="H19:H22"/>
-    <mergeCell ref="I19:I22"/>
-    <mergeCell ref="J19:J22"/>
-    <mergeCell ref="A15:A18"/>
-    <mergeCell ref="B15:B18"/>
-    <mergeCell ref="C15:C18"/>
-    <mergeCell ref="D15:D18"/>
-    <mergeCell ref="H15:H18"/>
-    <mergeCell ref="I15:I18"/>
-    <mergeCell ref="J7:J10"/>
-    <mergeCell ref="A11:A14"/>
-    <mergeCell ref="B11:B14"/>
-    <mergeCell ref="C11:C14"/>
-    <mergeCell ref="D11:D14"/>
-    <mergeCell ref="H11:H14"/>
-    <mergeCell ref="I11:I14"/>
-    <mergeCell ref="J11:J14"/>
-    <mergeCell ref="A7:A10"/>
-    <mergeCell ref="B7:B10"/>
-    <mergeCell ref="C7:C10"/>
-    <mergeCell ref="D7:D10"/>
-    <mergeCell ref="H7:H10"/>
-    <mergeCell ref="I7:I10"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="J1:J2"/>
     <mergeCell ref="A3:A6"/>
@@ -1467,6 +1395,48 @@
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="E1:G1"/>
     <mergeCell ref="H1:H2"/>
+    <mergeCell ref="J7:J10"/>
+    <mergeCell ref="A11:A14"/>
+    <mergeCell ref="B11:B14"/>
+    <mergeCell ref="C11:C14"/>
+    <mergeCell ref="D11:D14"/>
+    <mergeCell ref="H11:H14"/>
+    <mergeCell ref="I11:I14"/>
+    <mergeCell ref="J11:J14"/>
+    <mergeCell ref="A7:A10"/>
+    <mergeCell ref="B7:B10"/>
+    <mergeCell ref="C7:C10"/>
+    <mergeCell ref="D7:D10"/>
+    <mergeCell ref="H7:H10"/>
+    <mergeCell ref="I7:I10"/>
+    <mergeCell ref="J15:J18"/>
+    <mergeCell ref="A19:A22"/>
+    <mergeCell ref="B19:B22"/>
+    <mergeCell ref="C19:C22"/>
+    <mergeCell ref="D19:D22"/>
+    <mergeCell ref="H19:H22"/>
+    <mergeCell ref="I19:I22"/>
+    <mergeCell ref="J19:J22"/>
+    <mergeCell ref="A15:A18"/>
+    <mergeCell ref="B15:B18"/>
+    <mergeCell ref="C15:C18"/>
+    <mergeCell ref="D15:D18"/>
+    <mergeCell ref="H15:H18"/>
+    <mergeCell ref="I15:I18"/>
+    <mergeCell ref="J23:J26"/>
+    <mergeCell ref="A27:A30"/>
+    <mergeCell ref="B27:B30"/>
+    <mergeCell ref="C27:C30"/>
+    <mergeCell ref="D27:D30"/>
+    <mergeCell ref="H27:H30"/>
+    <mergeCell ref="I27:I30"/>
+    <mergeCell ref="J27:J30"/>
+    <mergeCell ref="A23:A26"/>
+    <mergeCell ref="B23:B26"/>
+    <mergeCell ref="C23:C26"/>
+    <mergeCell ref="D23:D26"/>
+    <mergeCell ref="H23:H26"/>
+    <mergeCell ref="I23:I26"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" sqref="J3 J7 J11 J15 J19 J23 J27">

</xml_diff>